<commit_message>
Two Pointers Array Questions
</commit_message>
<xml_diff>
--- a/Leetcode/DSA/Excel Notes.xlsx
+++ b/Leetcode/DSA/Excel Notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="1101">
   <si>
     <t>No.</t>
   </si>
@@ -3935,6 +3935,39 @@
   </si>
   <si>
     <t>Return sb.toString().trim().</t>
+  </si>
+  <si>
+    <t>keep a sum variable and iterate over the array, incrementing the sum with each element ans assigning sum at each indices in the array</t>
+  </si>
+  <si>
+    <t>iterate over the array and if any element is not 0 move it to first empty position of the array, use i=0 and j=0, again iterate and fill the remaining empty fields of array with 0</t>
+  </si>
+  <si>
+    <t>Max Number of K-Sum Pairs</t>
+  </si>
+  <si>
+    <t>Two pointers</t>
+  </si>
+  <si>
+    <t>create a count=0 variable and a Hashmap map, iterate the input array, if(map.getOrDefault(k-nums[i],0) &gt; 0), then increment the count, and decrement the frequency else, increment the freq of nums[i].</t>
+  </si>
+  <si>
+    <t>Sort the input array, put 1st pointer i=0 and 2nd pointer j= nums.length-1. Now using while loop until i&lt;j, keep checking for the value of the sum. Return count</t>
+  </si>
+  <si>
+    <t>Return count</t>
+  </si>
+  <si>
+    <t>Container with most water</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>Create a maxArea=min_value, variable, put 1st pointer i=0 and 2nd pointer j= nums.length-1. while(i&lt;j), keep checking the area of nums[i] and nums[j] and update the maxArea with calculated area.</t>
+  </si>
+  <si>
+    <t>If(height[i]&lt;=height[j]){i++;}else{j--;} Return maxArea</t>
   </si>
 </sst>
 </file>
@@ -8716,10 +8749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="F30" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8854,7 +8887,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>151</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -8874,7 +8907,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -9216,6 +9249,85 @@
     <row r="37" spans="1:7">
       <c r="G37" t="s">
         <v>1083</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E39" t="s">
+        <v>207</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="G40" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="G42" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="G43" s="8" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="B45">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="G46" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="G47" t="s">
+        <v>1100</v>
       </c>
     </row>
   </sheetData>
@@ -9228,7 +9340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sliding Window, Prefix Sum
</commit_message>
<xml_diff>
--- a/Leetcode/DSA/Excel Notes.xlsx
+++ b/Leetcode/DSA/Excel Notes.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="1121">
   <si>
     <t>No.</t>
   </si>
@@ -3919,9 +3919,6 @@
     <t>In res[] array, add the product of suffix and prefix at that particular index. Return res array.</t>
   </si>
   <si>
-    <t>Mediumm</t>
-  </si>
-  <si>
     <t>Reverse Words in a String</t>
   </si>
   <si>
@@ -3968,13 +3965,76 @@
   </si>
   <si>
     <t>If(height[i]&lt;=height[j]){i++;}else{j--;} Return maxArea</t>
+  </si>
+  <si>
+    <t>Maximum Average Subarray 1</t>
+  </si>
+  <si>
+    <t>We keep a window of k, for first k elements we calculate sum, now we start a loop for elements just after first k till n-1. Here we add current element to the sum variable and substract (i-kth) element.</t>
+  </si>
+  <si>
+    <t>Keep a maxAvg  and avg to calculate maxAvg for each i, return (double)maxAvg/k.</t>
+  </si>
+  <si>
+    <t>Maximum number of vowels in a substring of given length</t>
+  </si>
+  <si>
+    <t>Use a Hashset to store all 5 vowels. Calculate vowels for first k elements. Now iterate for remaining for i=k to i=n-1, check in set for each index i if character is a vowel, if it is, then increment the vowel variable by 1.</t>
+  </si>
+  <si>
+    <t>Also check in set at each index (i-k) if character it is, if it is, decrement the vowel variable by 1. Use a maxVowel variable to calculate maxVowels at each index. Return maxVowel.</t>
+  </si>
+  <si>
+    <t>Max Consecutives Ones 3</t>
+  </si>
+  <si>
+    <t>Here, we need to have a flexible window size. We will only flip a zero if it extends an existing window of 1s. We can never have &gt; K zeros. The way to shrink or expand a window would be based on the</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> number of zeros that can still be flipped and so on.</t>
+  </si>
+  <si>
+    <t>Create variable i=0,j=0, numZeroes=0,maxZeroes=0. Iterate using while loop until j&lt;nums.length. In iteration if an element is 0, increment numZeroes by 1. While(numZeroes&gt;k) if first element of window</t>
+  </si>
+  <si>
+    <t>nums[i]==0, decrement numZeroes. Change window size as i++. Calculate maxAvg using maxOnes = Math.max(maxOnes,j-i+1) just outside of 2nd while loop. Increment window side, j++,Return maxOnes.</t>
+  </si>
+  <si>
+    <t>Longest Subarray if 1's After Deleting One Elem</t>
+  </si>
+  <si>
+    <t>Maintain a sliding window where there is at most one zero on it.</t>
+  </si>
+  <si>
+    <t>Use above problem solution, k will be replaced by 1, j-i+1 will be replaced by j-i.</t>
+  </si>
+  <si>
+    <t>Prefix Sum</t>
+  </si>
+  <si>
+    <t>Find the Highest Altitude</t>
+  </si>
+  <si>
+    <t>You are given an integer array gain of length n where gain[i] is the net gain in altitude between points i​​​​​​ and i + 1 for all (0 &lt;= i &lt; n).</t>
+  </si>
+  <si>
+    <t>Since, starting at 0th point which has altitude 0. Create currAltitude=0 and highestAltitude=currAltitude. Now, since is element gain[i] in the array is the net gain in altitude between points I and i+1.</t>
+  </si>
+  <si>
+    <t>Thus we can calculate the height of one point by adding the altitude of previous point and net gain. Thus, using running sum and maxAlt we can calculate maximu Altitude.</t>
+  </si>
+  <si>
+    <t>We need a sum=0 and leftSum=0 variable, store sum of array in sum variable using for loop. Now use another for loop from i=0 to i=n-1. For each iteration check if (sum-leftSum-nums[i] == leftSum)</t>
+  </si>
+  <si>
+    <t>if it is, return i. increment leftSum += nums[i]. Outside of loop, return -1.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4146,6 +4206,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4168,7 +4235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4204,6 +4271,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4487,7 +4555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H300"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
@@ -8749,10 +8817,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F30" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8887,7 +8955,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -8907,7 +8975,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -9262,7 +9330,7 @@
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E39" t="s">
         <v>207</v>
@@ -9271,12 +9339,12 @@
         <v>10</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="G40" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -9292,15 +9360,18 @@
     </row>
     <row r="42" spans="1:7">
       <c r="G42" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="G43" s="8" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
       <c r="B45">
         <v>21</v>
       </c>
@@ -9308,7 +9379,7 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E45" t="s">
         <v>9</v>
@@ -9317,17 +9388,197 @@
         <v>10</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="G46" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="G47" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
         <v>1100</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="G50" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="G51" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="G54" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="G55" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="G56" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="G57" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="G60" s="29" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="G61" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B63">
+        <v>25</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="G64" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="G65" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="G66" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B68">
+        <v>26</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>124</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="G69" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="G70" t="s">
+        <v>1120</v>
       </c>
     </row>
   </sheetData>
@@ -9338,16 +9589,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="7" max="7" width="172.5546875" customWidth="1"/>
   </cols>
@@ -9521,10 +9772,10 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
         <v>1084</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1085</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -9533,22 +9784,55 @@
         <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="G19" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="G20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="G21" t="s">
-        <v>1089</v>
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="G24" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="G25" t="s">
+        <v>1105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Equal Row and Column Pairs
</commit_message>
<xml_diff>
--- a/Leetcode/DSA/Excel Notes.xlsx
+++ b/Leetcode/DSA/Excel Notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2148" uniqueCount="1132">
   <si>
     <t>No.</t>
   </si>
@@ -4052,6 +4052,15 @@
   </si>
   <si>
     <t xml:space="preserve">Now considering above 3 points we can formulate our code. </t>
+  </si>
+  <si>
+    <t>Equal Row and Column Pairs</t>
+  </si>
+  <si>
+    <t>Here, we need to compare each row with each column. Thus we can iterate over 2d array normally and append each row as string in hashmap. Now, similarily, we can convert each column in string</t>
+  </si>
+  <si>
+    <t>and check whether that string column hashmap already contains. If it does, we increment a count variable by value of that string key and return count</t>
   </si>
 </sst>
 </file>
@@ -8841,10 +8850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="E47" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9605,6 +9614,39 @@
         <v>1120</v>
       </c>
     </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B72">
+        <v>27</v>
+      </c>
+      <c r="C72" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E72" t="s">
+        <v>36</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="G73" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="G74" t="s">
+        <v>1131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9615,7 +9657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+    <sheetView topLeftCell="E7" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>

</xml_diff>